<commit_message>
Implemented Ca40 input file
</commit_message>
<xml_diff>
--- a/input_files/O16_RMF.xlsx
+++ b/input_files/O16_RMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Projects/Light-Front Mean Field Theory/Runge-Kutta Method/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB980500-198F-ED45-A338-AFE8D71D6F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6385EA1-61C4-A24B-BFA4-B933A3A2F6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="2480" windowWidth="28800" windowHeight="15640" xr2:uid="{178560A9-F361-274A-AB9D-3DA0C106A5E5}"/>
+    <workbookView xWindow="5940" yWindow="2660" windowWidth="28800" windowHeight="15640" activeTab="3" xr2:uid="{178560A9-F361-274A-AB9D-3DA0C106A5E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9A6784-E59C-C844-8BF2-222A93D550FE}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -529,15 +529,15 @@
         <v>770</v>
       </c>
       <c r="E2">
-        <f>0.0000001</f>
-        <v>9.9999999999999995E-8</v>
+        <f>0.04</f>
+        <v>0.04</v>
       </c>
       <c r="F2">
         <f>12</f>
         <v>12</v>
       </c>
       <c r="G2">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +550,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,12 +589,12 @@
         <v>410</v>
       </c>
       <c r="C2">
-        <f>SQRT(109.6)</f>
-        <v>10.469001862641921</v>
+        <f>SQRT(109.6264)</f>
+        <v>10.470262651910888</v>
       </c>
       <c r="D2">
-        <f>SQRT(190.4)</f>
-        <v>13.798550648528272</v>
+        <f>SQRT(190.4306)</f>
+        <v>13.799659416087051</v>
       </c>
       <c r="E2">
         <v>3.6</v>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF253CE-956B-B040-8027-78DFB140BDDF}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>